<commit_message>
Updated the unit tests for web-work to eliminate HED-2G tests
</commit_message>
<xml_diff>
--- a/webtools/tests/data/ExcelMultipleSheets.xlsx
+++ b/webtools/tests/data/ExcelMultipleSheets.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\HEDPython\hed-python\webtools\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEDPython\hed-python\webtools\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LKT 8HED3" sheetId="4" r:id="rId1"/>
     <sheet name="LKT Events" sheetId="1" r:id="rId2"/>
     <sheet name="PVT Events" sheetId="2" r:id="rId3"/>
     <sheet name="DAS Events" sheetId="3" r:id="rId4"/>
+    <sheet name="LKT 8HED3A" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
   <si>
     <t>Event code</t>
   </si>
@@ -676,7 +677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1118,4 +1119,112 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6"/>
+  <cols>
+    <col min="1" max="1" width="15.3828125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="23.07421875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="57.3828125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="41.921875" style="2" customWidth="1"/>
+    <col min="6" max="1026" width="8.53515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="43.75">
+      <c r="A2" s="1">
+        <v>251</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.75">
+      <c r="A3" s="1">
+        <v>252</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="47.05" customHeight="1">
+      <c r="A4" s="1">
+        <v>253</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.75">
+      <c r="A5" s="1">
+        <v>254</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
 </file>
</xml_diff>